<commit_message>
pom last class changes
</commit_message>
<xml_diff>
--- a/TestInput/OHRMS_Input.xlsx
+++ b/TestInput/OHRMS_Input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>TC_Name</t>
   </si>
@@ -34,18 +34,12 @@
     <t>Hannah Flores</t>
   </si>
   <si>
-    <t>Donald Trump</t>
-  </si>
-  <si>
     <t>America123#</t>
   </si>
   <si>
     <t>AssignLeave</t>
   </si>
   <si>
-    <t>Jasmine Morgan</t>
-  </si>
-  <si>
     <t>LeaveType</t>
   </si>
   <si>
@@ -79,7 +73,10 @@
     <t>Donald</t>
   </si>
   <si>
-    <t xml:space="preserve"> Trump</t>
+    <t>Donald Trump1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trump1</t>
   </si>
 </sst>
 </file>
@@ -415,7 +412,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -448,50 +445,50 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
       <c r="G3" s="1">
         <v>43979</v>
@@ -500,18 +497,18 @@
         <v>44071</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>